<commit_message>
Refining code for experimentation
</commit_message>
<xml_diff>
--- a/Rubric_project/Data/Learner_Profile_8_Jan_2025.xlsx
+++ b/Rubric_project/Data/Learner_Profile_8_Jan_2025.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
   <si>
     <t xml:space="preserve">Learner</t>
   </si>
@@ -161,18 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">[19, 26, 31, 35, 38]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MS Electrical Engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[2, 2, 2, 2, 1, 1, 1, 2, 2, 1, 1, 1, 1, 1, 1, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 2, 1, 2, 1, 2, 2, 2, 2, 2, 2, 2, 2, 1, 1, 1, 1, 1, 1, 1, 1, 1, 2, 2, 1, 1, 2, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[]</t>
   </si>
   <si>
     <t xml:space="preserve">Student 8</t>
@@ -449,10 +437,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,7 +448,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="132.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="60.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.33"/>
   </cols>
   <sheetData>
@@ -876,37 +864,37 @@
         <v>34</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K8" s="1" t="n">
         <v>9</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O8" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P8" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="Q8" s="1" t="n">
-        <v>60</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>43</v>
@@ -920,49 +908,49 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>43</v>
@@ -970,13 +958,13 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>56</v>
@@ -988,10 +976,10 @@
         <v>34</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>6</v>
@@ -1000,19 +988,19 @@
         <v>4</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O10" s="1" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P10" s="1" t="n">
         <v>30</v>
@@ -1021,7 +1009,7 @@
         <v>90</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,37 +1035,37 @@
         <v>8</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P11" s="1" t="n">
         <v>30</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,28 +1088,28 @@
         <v>34</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L12" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1" t="n">
         <v>7</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O12" s="1" t="n">
         <v>9</v>
@@ -1133,7 +1121,7 @@
         <v>120</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,98 +1144,43 @@
         <v>34</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O13" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="K14" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="L14" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="M14" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="N14" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="O14" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="P14" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q14" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="R14" s="1" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>